<commit_message>
tidy sweeping gap analysis
</commit_message>
<xml_diff>
--- a/sweeping_gap/sweeping_gap_results_summary.xlsx
+++ b/sweeping_gap/sweeping_gap_results_summary.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="16">
   <si>
     <t xml:space="preserve">Reference: </t>
   </si>
@@ -87,6 +87,9 @@
   </si>
   <si>
     <t>LA7 ImageJ:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Test </t>
   </si>
 </sst>
 </file>
@@ -153,11 +156,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -169,6 +169,12 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -453,417 +459,422 @@
   <dimension ref="B1:K37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F37" sqref="F37"/>
+      <selection activeCell="C46" sqref="C46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="11" width="20.7109375" customWidth="1"/>
+    <col min="2" max="6" width="20.7109375" customWidth="1"/>
+    <col min="7" max="7" width="2.7109375" customWidth="1"/>
+    <col min="8" max="11" width="20.7109375" customWidth="1"/>
     <col min="12" max="12" width="2.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:11" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B1" s="6" t="s">
+    <row r="1" spans="2:11" ht="61.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
-      <c r="F1" s="1"/>
-      <c r="G1" s="1"/>
-      <c r="H1" s="1"/>
-      <c r="I1" s="1"/>
-      <c r="J1" s="1"/>
-      <c r="K1" s="1"/>
+      <c r="D1" s="7"/>
+      <c r="E1" s="7"/>
+      <c r="F1" s="7"/>
+      <c r="G1" s="8"/>
+      <c r="H1" s="8"/>
+      <c r="I1" s="8"/>
+      <c r="J1" s="8"/>
+      <c r="K1" s="8"/>
     </row>
     <row r="3" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B3" s="6" t="s">
+      <c r="B3" s="5" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="5" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B5" s="2"/>
-      <c r="C5" s="3" t="s">
+      <c r="B5" s="1"/>
+      <c r="C5" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="D5" s="3" t="s">
+      <c r="D5" s="2" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="6" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B6" s="2" t="s">
+      <c r="B6" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C6" s="4">
+      <c r="C6" s="3">
         <v>1.19</v>
       </c>
-      <c r="D6" s="4">
+      <c r="D6" s="3">
         <v>1.03</v>
       </c>
     </row>
     <row r="7" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B7" s="2" t="s">
+      <c r="B7" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C7" s="4">
+      <c r="C7" s="3">
         <v>0.44</v>
       </c>
-      <c r="D7" s="4">
+      <c r="D7" s="3">
         <v>0.43</v>
       </c>
     </row>
     <row r="8" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B8" s="2" t="s">
+      <c r="B8" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C8" s="4">
+      <c r="C8" s="3">
         <v>1.19</v>
       </c>
-      <c r="D8" s="4">
+      <c r="D8" s="3">
         <v>1.05</v>
       </c>
     </row>
     <row r="9" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B9" s="2" t="s">
+      <c r="B9" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C9" s="4">
+      <c r="C9" s="3">
         <v>0.12</v>
       </c>
-      <c r="D9" s="4">
+      <c r="D9" s="3">
         <v>0.12</v>
       </c>
     </row>
     <row r="10" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B10" s="2" t="s">
+      <c r="B10" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C10" s="4">
+      <c r="C10" s="3">
         <v>0.47</v>
       </c>
-      <c r="D10" s="4">
+      <c r="D10" s="3">
         <v>0.41</v>
       </c>
     </row>
     <row r="12" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B12" s="5" t="s">
+      <c r="B12" s="4" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="14" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B14" s="2"/>
-      <c r="C14" s="3" t="s">
+      <c r="B14" s="1"/>
+      <c r="C14" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="D14" s="3" t="s">
+      <c r="D14" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="E14" s="3" t="s">
+      <c r="E14" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="F14" s="3" t="s">
+      <c r="F14" s="2" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="15" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B15" s="2" t="s">
+      <c r="B15" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C15" s="7">
+      <c r="C15" s="6">
         <v>1.1000000000000001</v>
       </c>
-      <c r="D15" s="7">
+      <c r="D15" s="6">
         <v>0.99</v>
       </c>
-      <c r="E15" s="7">
+      <c r="E15" s="6">
         <v>1.31</v>
       </c>
-      <c r="F15" s="7">
+      <c r="F15" s="6">
         <v>1.18</v>
       </c>
     </row>
     <row r="16" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B16" s="2" t="s">
+      <c r="B16" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C16" s="7" t="str">
-        <f>"-"</f>
-        <v>-</v>
-      </c>
-      <c r="D16" s="7">
+      <c r="C16" s="6" t="str">
+        <f>"-"</f>
+        <v>-</v>
+      </c>
+      <c r="D16" s="6">
         <v>0.65</v>
       </c>
-      <c r="E16" s="7" t="str">
-        <f>"-"</f>
-        <v>-</v>
-      </c>
-      <c r="F16" s="7">
+      <c r="E16" s="6" t="str">
+        <f>"-"</f>
+        <v>-</v>
+      </c>
+      <c r="F16" s="6">
         <v>0.74</v>
       </c>
     </row>
     <row r="17" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B17" s="2" t="s">
+      <c r="B17" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C17" s="7" t="str">
-        <f>"-"</f>
-        <v>-</v>
-      </c>
-      <c r="D17" s="7">
+      <c r="C17" s="6" t="str">
+        <f>"-"</f>
+        <v>-</v>
+      </c>
+      <c r="D17" s="6">
         <v>0.53</v>
       </c>
-      <c r="E17" s="7" t="str">
-        <f>"-"</f>
-        <v>-</v>
-      </c>
-      <c r="F17" s="7">
+      <c r="E17" s="6" t="str">
+        <f>"-"</f>
+        <v>-</v>
+      </c>
+      <c r="F17" s="6">
         <v>0.52</v>
       </c>
     </row>
     <row r="18" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B18" s="2" t="s">
+      <c r="B18" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C18" s="7" t="str">
-        <f>"-"</f>
-        <v>-</v>
-      </c>
-      <c r="D18" s="7">
+      <c r="C18" s="6" t="str">
+        <f>"-"</f>
+        <v>-</v>
+      </c>
+      <c r="D18" s="6">
         <v>0.13</v>
       </c>
-      <c r="E18" s="7" t="str">
-        <f>"-"</f>
-        <v>-</v>
-      </c>
-      <c r="F18" s="7">
+      <c r="E18" s="6" t="str">
+        <f>"-"</f>
+        <v>-</v>
+      </c>
+      <c r="F18" s="6">
         <v>0.18</v>
       </c>
     </row>
     <row r="19" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B19" s="2" t="s">
+      <c r="B19" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C19" s="7">
+      <c r="C19" s="6">
         <v>0.44</v>
       </c>
-      <c r="D19" s="7">
+      <c r="D19" s="6">
         <v>0.38</v>
       </c>
-      <c r="E19" s="7">
+      <c r="E19" s="6">
         <v>0.57999999999999996</v>
       </c>
-      <c r="F19" s="7">
+      <c r="F19" s="6">
         <v>0.5</v>
       </c>
     </row>
     <row r="21" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B21" s="5" t="s">
+      <c r="B21" s="4" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="23" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B23" s="2"/>
-      <c r="C23" s="3" t="s">
+      <c r="B23" s="1"/>
+      <c r="C23" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="D23" s="3" t="s">
+      <c r="D23" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="E23" s="3" t="s">
+      <c r="E23" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="F23" s="3" t="s">
+      <c r="F23" s="2" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="24" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B24" s="2" t="s">
+      <c r="B24" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C24" s="7">
+      <c r="C24" s="6">
         <v>0.95</v>
       </c>
-      <c r="D24" s="7">
+      <c r="D24" s="6">
         <v>0.48</v>
       </c>
-      <c r="E24" s="7" t="str">
-        <f>"-"</f>
-        <v>-</v>
-      </c>
-      <c r="F24" s="7">
+      <c r="E24" s="6" t="str">
+        <f>"-"</f>
+        <v>-</v>
+      </c>
+      <c r="F24" s="6">
         <v>0.87</v>
       </c>
     </row>
     <row r="25" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B25" s="2" t="s">
+      <c r="B25" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C25" s="7"/>
-      <c r="D25" s="7"/>
-      <c r="E25" s="7" t="str">
-        <f>"-"</f>
-        <v>-</v>
-      </c>
-      <c r="F25" s="7">
+      <c r="C25" s="6"/>
+      <c r="D25" s="6"/>
+      <c r="E25" s="6" t="str">
+        <f>"-"</f>
+        <v>-</v>
+      </c>
+      <c r="F25" s="6">
         <v>0.54</v>
       </c>
     </row>
     <row r="26" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B26" s="2" t="s">
+      <c r="B26" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C26" s="7"/>
-      <c r="D26" s="7"/>
-      <c r="E26" s="7" t="str">
-        <f>"-"</f>
-        <v>-</v>
-      </c>
-      <c r="F26" s="7">
+      <c r="C26" s="6"/>
+      <c r="D26" s="6"/>
+      <c r="E26" s="6" t="str">
+        <f>"-"</f>
+        <v>-</v>
+      </c>
+      <c r="F26" s="6">
         <v>0.56999999999999995</v>
       </c>
     </row>
     <row r="27" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B27" s="2" t="s">
+      <c r="B27" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C27" s="7"/>
-      <c r="D27" s="7"/>
-      <c r="E27" s="7" t="str">
-        <f>"-"</f>
-        <v>-</v>
-      </c>
-      <c r="F27" s="7">
+      <c r="C27" s="6"/>
+      <c r="D27" s="6"/>
+      <c r="E27" s="6" t="str">
+        <f>"-"</f>
+        <v>-</v>
+      </c>
+      <c r="F27" s="6">
         <v>0.1</v>
       </c>
     </row>
     <row r="28" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B28" s="2" t="s">
+      <c r="B28" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C28" s="7">
+      <c r="C28" s="6">
         <v>0.28999999999999998</v>
       </c>
-      <c r="D28" s="7">
+      <c r="D28" s="6">
         <v>0</v>
       </c>
-      <c r="E28" s="7" t="str">
-        <f>"-"</f>
-        <v>-</v>
-      </c>
-      <c r="F28" s="7">
+      <c r="E28" s="6" t="str">
+        <f>"-"</f>
+        <v>-</v>
+      </c>
+      <c r="F28" s="6">
         <v>0.28999999999999998</v>
       </c>
     </row>
     <row r="30" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B30" s="5" t="s">
+      <c r="B30" s="4" t="s">
         <v>14</v>
       </c>
+      <c r="C30" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="32" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B32" s="2"/>
-      <c r="C32" s="3" t="s">
+      <c r="B32" s="1"/>
+      <c r="C32" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="D32" s="3" t="s">
+      <c r="D32" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="E32" s="3" t="s">
+      <c r="E32" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="F32" s="3" t="s">
+      <c r="F32" s="2" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="33" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B33" s="2" t="s">
+      <c r="B33" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C33" s="7">
+      <c r="C33" s="6">
         <v>0.87</v>
       </c>
-      <c r="D33" s="7">
+      <c r="D33" s="6">
         <v>0.56000000000000005</v>
       </c>
-      <c r="E33" s="7">
+      <c r="E33" s="6">
         <v>1.27</v>
       </c>
-      <c r="F33" s="7">
+      <c r="F33" s="6">
         <v>1.2</v>
       </c>
     </row>
     <row r="34" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B34" s="2" t="s">
+      <c r="B34" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C34" s="7">
+      <c r="C34" s="6">
         <v>0.56999999999999995</v>
       </c>
-      <c r="D34" s="7">
+      <c r="D34" s="6">
         <v>0.55000000000000004</v>
       </c>
-      <c r="E34" s="7">
+      <c r="E34" s="6">
         <v>0.56999999999999995</v>
       </c>
-      <c r="F34" s="7">
+      <c r="F34" s="6">
         <v>0.56000000000000005</v>
       </c>
     </row>
     <row r="35" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B35" s="2" t="s">
+      <c r="B35" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C35" s="7">
+      <c r="C35" s="6">
         <v>0.56999999999999995</v>
       </c>
-      <c r="D35" s="7">
+      <c r="D35" s="6">
         <v>0.39</v>
       </c>
-      <c r="E35" s="7">
+      <c r="E35" s="6">
         <v>0.61</v>
       </c>
-      <c r="F35" s="7">
+      <c r="F35" s="6">
         <v>0.55000000000000004</v>
       </c>
     </row>
     <row r="36" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B36" s="2" t="s">
+      <c r="B36" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C36" s="7">
+      <c r="C36" s="6">
         <v>0.02</v>
       </c>
-      <c r="D36" s="7">
+      <c r="D36" s="6">
         <v>0.03</v>
       </c>
-      <c r="E36" s="7">
+      <c r="E36" s="6">
         <v>8.9999999999999993E-3</v>
       </c>
-      <c r="F36" s="7">
+      <c r="F36" s="6">
         <v>0.01</v>
       </c>
     </row>
     <row r="37" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B37" s="2" t="s">
+      <c r="B37" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C37" s="7">
+      <c r="C37" s="6">
         <v>0.13</v>
       </c>
-      <c r="D37" s="7">
+      <c r="D37" s="6">
         <v>-0.12</v>
       </c>
-      <c r="E37" s="7">
+      <c r="E37" s="6">
         <v>0.31</v>
       </c>
-      <c r="F37" s="7">
+      <c r="F37" s="6">
         <v>0.13</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="C1:K1"/>
+    <mergeCell ref="C1:F1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>